<commit_message>
remove links for atomic file validation
</commit_message>
<xml_diff>
--- a/02-Dataset2_MEP/04-SHACL/Dataset2_MEP-Shapes.xlsx
+++ b/02-Dataset2_MEP/04-SHACL/Dataset2_MEP-Shapes.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\00-Clients\EP\20-Repository\ep-graph-poc\02-Dataset2_MEP\04-SHACL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{284F34AE-CA35-4FD1-84A7-787FBE16790E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A66E8685-EB26-45BC-8FDD-20C33869435B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="26940" windowHeight="13395" tabRatio="994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="26940" windowHeight="13395" tabRatio="994" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="class-based shapes" sheetId="1" r:id="rId1"/>
@@ -500,7 +500,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -523,6 +523,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF729FCF"/>
         <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -589,10 +595,10 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -978,7 +984,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMK21"/>
   <sheetViews>
-    <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView windowProtection="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -1162,7 +1168,7 @@
       <c r="B10" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="22" t="s">
+      <c r="D10" s="21" t="s">
         <v>86</v>
       </c>
       <c r="E10" s="1" t="s">
@@ -1252,7 +1258,7 @@
       <c r="B13" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="22" t="s">
+      <c r="D13" s="21" t="s">
         <v>124</v>
       </c>
       <c r="E13" s="1" t="s">
@@ -1327,9 +1333,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMN39"/>
   <sheetViews>
-    <sheetView windowProtection="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
+    <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="8" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1774,7 +1780,7 @@
       <c r="H20">
         <v>1</v>
       </c>
-      <c r="J20" s="21" t="s">
+      <c r="J20" s="22" t="s">
         <v>93</v>
       </c>
       <c r="L20" t="s">
@@ -2095,7 +2101,7 @@
       <c r="H39">
         <v>1</v>
       </c>
-      <c r="J39" s="21" t="s">
+      <c r="J39" s="22" t="s">
         <v>61</v>
       </c>
       <c r="L39" t="s">

</xml_diff>

<commit_message>
Update constraints on URI of Dataset2
</commit_message>
<xml_diff>
--- a/02-Dataset2_MEP/04-SHACL/Dataset2_MEP-Shapes.xlsx
+++ b/02-Dataset2_MEP/04-SHACL/Dataset2_MEP-Shapes.xlsx
@@ -157,7 +157,34 @@
 (toujours mettre /1 à la fin)</t>
   </si>
   <si>
-    <t xml:space="preserve">"^http://data.europarl.europa.eu/person/MEP_[0-9][0-9][0-9][0-9]?[0-9]?[0-9]?/membership/[0-9]$"</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">"^</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">http://data.europarl.europa.eu/person/MEP_[0-9][0-9][0-9][0-9]?[0-9]?[0-9]?/membership/[0-9][0-9]?[0-9]?[0-9]?[0-9]?$</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">"</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">epsh:PoliticalGroup</t>
@@ -761,11 +788,11 @@
   </sheetPr>
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I12" activeCellId="0" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.4609375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.58"/>
@@ -943,7 +970,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="57.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>39</v>
       </c>
@@ -966,7 +993,7 @@
       <c r="H11" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I11" s="15" t="s">
+      <c r="I11" s="0" t="s">
         <v>43</v>
       </c>
       <c r="J11" s="1" t="s">
@@ -1104,7 +1131,7 @@
     <hyperlink ref="B1" r:id="rId1" display="http://data.europarl.europa.eu/shapes"/>
     <hyperlink ref="E9" r:id="rId2" display="rdfs:label@fr"/>
     <hyperlink ref="G9" r:id="rId3" display="rdfs:comment@fr"/>
-    <hyperlink ref="I11" r:id="rId4" display="&quot;^http://data.europarl.europa.eu/person/MEP_[0-9][0-9][0-9][0-9]?[0-9]?[0-9]?/membership/[0-9]$&quot;"/>
+    <hyperlink ref="I11" r:id="rId4" display="http://data.europarl.europa.eu/person/MEP_[0-9][0-9][0-9][0-9]?[0-9]?[0-9]?/membership/[0-9][0-9]?[0-9]?[0-9]?[0-9]?$"/>
     <hyperlink ref="I12" r:id="rId5" display="&quot;^http://data.europarl.europa.eu/org/group/.*$&quot;"/>
     <hyperlink ref="I14" r:id="rId6" display="&quot;^http://data.europarl.europa.eu/person/Assistant_[0-9][0-9][0-9][0-9][0-9]?[0-9]?/membership/[0-9]$&quot;"/>
   </hyperlinks>
@@ -1131,7 +1158,7 @@
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.61328125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.99"/>

</xml_diff>

<commit_message>
Update of SHACL files with description/comments
</commit_message>
<xml_diff>
--- a/02-Dataset2_MEP/04-SHACL/Dataset2_MEP-Shapes.xlsx
+++ b/02-Dataset2_MEP/04-SHACL/Dataset2_MEP-Shapes.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="157">
   <si>
     <t xml:space="preserve">Shapes URI</t>
   </si>
@@ -113,7 +113,7 @@
     <t xml:space="preserve">sh:order^^xsd:integer</t>
   </si>
   <si>
-    <t xml:space="preserve">rdfs:comment@fr</t>
+    <t xml:space="preserve">rdfs:comment@en</t>
   </si>
   <si>
     <t xml:space="preserve">sh:nodeKind</t>
@@ -140,9 +140,8 @@
     <t xml:space="preserve">MEP</t>
   </si>
   <si>
-    <t xml:space="preserve">/person/{person id } 
-Example
-/person/MEP_342 </t>
+    <t xml:space="preserve">A Member of European Parliament. Example URI "
+/person/MEP_342"</t>
   </si>
   <si>
     <t xml:space="preserve">sh:IRI</t>
@@ -169,10 +168,7 @@
     <t xml:space="preserve">MEP political party membership</t>
   </si>
   <si>
-    <t xml:space="preserve">person/{id  }/membership/{serial}
-Example
-person/MEP_342/membership/1
-(toujours mettre /1 à la fin)</t>
+    <t xml:space="preserve">A relation between MEP and the political group (s)he belongs to at a given point in time. Example URI "person/MEP_342/membership/1"</t>
   </si>
   <si>
     <t xml:space="preserve">"^http://data.europarl.europa.eu/person/MEP_[0-9][0-9][0-9][0-9]?[0-9]?[0-9]?/membership/[0-9][0-9]?[0-9]?[0-9]?[0-9]?$"</t>
@@ -190,9 +186,7 @@
     <t xml:space="preserve">Political Group</t>
   </si>
   <si>
-    <t xml:space="preserve">org/{org-type}/{natural identifier} 
-Example : 
-/org/group/CD-497</t>
+    <t xml:space="preserve">A Political Group. Example URI "/org/group/CD-497"</t>
   </si>
   <si>
     <t xml:space="preserve">"^http://data.europarl.europa.eu/org/group/.*$"</t>
@@ -207,9 +201,7 @@
     <t xml:space="preserve">Assistant</t>
   </si>
   <si>
-    <t xml:space="preserve">/person/{person id  } 
-Example
-/person/Assistant_45 </t>
+    <t xml:space="preserve">An assistant to an MEP. Example URI "/person/Assistant_45"</t>
   </si>
   <si>
     <t xml:space="preserve">"^http://data.europarl.europa.eu/person/Assistant_[0-9][0-9][0-9][0-9][0-9]?[0-9]?$"</t>
@@ -227,10 +219,7 @@
     <t xml:space="preserve">Assistant membership to an MEP</t>
   </si>
   <si>
-    <t xml:space="preserve">person/{id  }/membership/{serial}
-Example
-person/MEP_342/membership/1
-Mettre un numéro séquentiel dans les membership</t>
+    <t xml:space="preserve">A relation between an Assistant and its MEP. An assistant may assist more than 1 MEP. Example URI "person/Assistant_45/membership/1"</t>
   </si>
   <si>
     <t xml:space="preserve">"^http://data.europarl.europa.eu/person/Assistant_[0-9][0-9][0-9][0-9][0-9]?[0-9]?/membership/[0-9]$"</t>
@@ -425,6 +414,9 @@
     <t xml:space="preserve">political party</t>
   </si>
   <si>
+    <t xml:space="preserve">Theoretically points to Shape PoliticalGroup, but this constraint is removed when validating files, because MEP and Political Groups are in different source files</t>
+  </si>
+  <si>
     <t xml:space="preserve">type</t>
   </si>
   <si>
@@ -495,6 +487,9 @@
   </si>
   <si>
     <t xml:space="preserve">Contraintes sur les MembershipAssistant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Theoretically points to Shape MEP, but this constraint is removed when validating files, because Assistant and MEP are in different source files</t>
   </si>
   <si>
     <t xml:space="preserve">(org:Membership eponto:MembershipAssistant)</t>
@@ -507,7 +502,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -588,6 +583,11 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -658,7 +658,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -745,6 +745,10 @@
     </xf>
     <xf numFmtId="164" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -827,11 +831,11 @@
   </sheetPr>
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.58"/>
@@ -1009,7 +1013,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>35</v>
       </c>
@@ -1044,7 +1048,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>44</v>
       </c>
@@ -1079,7 +1083,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>50</v>
       </c>
@@ -1114,7 +1118,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>56</v>
       </c>
@@ -1149,7 +1153,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>61</v>
       </c>
@@ -1214,7 +1218,7 @@
     <hyperlink ref="B1" r:id="rId1" display="http://data.europarl.europa.eu/shapes/meps"/>
     <hyperlink ref="D11" r:id="rId2" display="rdfs:label@fr"/>
     <hyperlink ref="E11" r:id="rId3" display="rdfs:label@en"/>
-    <hyperlink ref="G11" r:id="rId4" display="rdfs:comment@fr"/>
+    <hyperlink ref="G11" r:id="rId4" display="comment@en"/>
     <hyperlink ref="I13" r:id="rId5" display="&quot;^http://data.europarl.europa.eu/person/MEP_[0-9][0-9][0-9][0-9]?[0-9]?[0-9]?/membership/[0-9][0-9]?[0-9]?[0-9]?[0-9]?$&quot;"/>
     <hyperlink ref="I14" r:id="rId6" display="&quot;^http://data.europarl.europa.eu/org/group/.*$&quot;"/>
     <hyperlink ref="I16" r:id="rId7" display="&quot;^http://data.europarl.europa.eu/person/Assistant_[0-9][0-9][0-9][0-9][0-9]?[0-9]?/membership/[0-9]$&quot;"/>
@@ -1236,13 +1240,13 @@
   </sheetPr>
   <dimension ref="A1:T41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="O1" activeCellId="0" sqref="O1"/>
-      <selection pane="bottomLeft" activeCell="V8" activeCellId="0" sqref="V8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="8" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="F41" activeCellId="0" sqref="F41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.65234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.99"/>
@@ -1721,7 +1725,7 @@
       </c>
       <c r="T20" s="20"/>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="str">
         <f aca="false">CONCATENATE("epsh:P",ROW(A21))</f>
         <v>epsh:P21</v>
@@ -1737,6 +1741,9 @@
       </c>
       <c r="E21" s="0" t="s">
         <v>129</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>130</v>
       </c>
       <c r="G21" s="1" t="n">
         <v>1</v>
@@ -1769,7 +1776,7 @@
         <v>2</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="G22" s="1" t="n">
         <v>2</v>
@@ -1781,12 +1788,12 @@
         <v>40</v>
       </c>
       <c r="Q22" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="24" s="19" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="19" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="T24" s="20"/>
     </row>
@@ -1805,7 +1812,7 @@
         <v>1</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G25" s="1" t="n">
         <v>1</v>
@@ -1826,7 +1833,7 @@
         <v>epsh:P26</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>50</v>
@@ -1835,7 +1842,7 @@
         <v>2</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G26" s="1" t="n">
         <v>24</v>
@@ -1847,13 +1854,13 @@
         <v>107</v>
       </c>
       <c r="M26" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="S26" s="0" t="s">
         <v>42</v>
       </c>
       <c r="T26" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1862,7 +1869,7 @@
         <v>epsh:P27</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>50</v>
@@ -1871,7 +1878,7 @@
         <v>3</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G27" s="1" t="n">
         <v>1</v>
@@ -1883,7 +1890,7 @@
         <v>107</v>
       </c>
       <c r="M27" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1892,7 +1899,7 @@
         <v>epsh:P28</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>50</v>
@@ -1901,7 +1908,7 @@
         <v>4</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="G28" s="1" t="n">
         <v>1</v>
@@ -1913,7 +1920,7 @@
         <v>107</v>
       </c>
       <c r="M28" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1922,7 +1929,7 @@
         <v>epsh:P29</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>50</v>
@@ -1931,7 +1938,7 @@
         <v>5</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="G29" s="1" t="n">
         <v>1</v>
@@ -1943,7 +1950,7 @@
         <v>107</v>
       </c>
       <c r="M29" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1952,7 +1959,7 @@
         <v>epsh:P30</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>50</v>
@@ -1961,7 +1968,7 @@
         <v>6</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="G30" s="1" t="n">
         <v>1</v>
@@ -1973,7 +1980,7 @@
         <v>107</v>
       </c>
       <c r="M30" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2008,7 +2015,7 @@
     </row>
     <row r="33" s="19" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="19" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="T33" s="20"/>
     </row>
@@ -2078,7 +2085,7 @@
         <v>epsh:P36</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>56</v>
@@ -2087,7 +2094,7 @@
         <v>3</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="G36" s="1" t="n">
         <v>1</v>
@@ -2102,7 +2109,7 @@
         <v>108</v>
       </c>
       <c r="Q36" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2123,7 +2130,7 @@
         <v>126</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="G37" s="1" t="n">
         <v>1</v>
@@ -2138,11 +2145,11 @@
     </row>
     <row r="39" s="19" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="19" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="T39" s="20"/>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="57.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="str">
         <f aca="false">CONCATENATE("epsh:P",ROW(A40))</f>
         <v>epsh:P40</v>
@@ -2158,6 +2165,9 @@
       </c>
       <c r="E40" s="0" t="s">
         <v>38</v>
+      </c>
+      <c r="F40" s="22" t="s">
+        <v>155</v>
       </c>
       <c r="G40" s="1" t="n">
         <v>1</v>
@@ -2190,7 +2200,7 @@
         <v>2</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="G41" s="1" t="n">
         <v>2</v>
@@ -2202,7 +2212,7 @@
         <v>40</v>
       </c>
       <c r="Q41" s="0" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>